<commit_message>
Update Colors.xlsx add pantone col
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagja\Desktop\DHS207_Introduction to Digital History\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C13560E-7B40-4FC1-A523-AA457DFFFB9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A8ABC-51FA-4924-A960-6C432D2CD2CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9400" xr2:uid="{91E5F28C-6291-45D4-8C0D-F3DDD27ECA86}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="6040" xr2:uid="{91E5F28C-6291-45D4-8C0D-F3DDD27ECA86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="384">
   <si>
     <t>곤색;담청색</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1987,13 +1987,278 @@
       </rPr>
       <t>⾊)</t>
     </r>
+  </si>
+  <si>
+    <t>Formular Guide 7404 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2008 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 382 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7499 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 930 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4017 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 714 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 4002 CP</t>
+  </si>
+  <si>
+    <t>Formular Guide 715 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 722 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7751 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2318 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 122 CP</t>
+  </si>
+  <si>
+    <t>Formular Guide 487 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2312 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7687 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2925 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 542 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7459 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 3258 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2101 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7683 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2374 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2378 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 3574 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7677 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7675 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 5275 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4131 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 7730 CP</t>
+  </si>
+  <si>
+    <t>Color Bridge 2257 CP</t>
+  </si>
+  <si>
+    <t>Extended Gamut 7739 XGC</t>
+  </si>
+  <si>
+    <t>Formular Guide 7737 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 374 C</t>
+  </si>
+  <si>
+    <t>Extended Gamut 2281 XGC</t>
+  </si>
+  <si>
+    <t>CMYK P 130-14 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2243 C</t>
+  </si>
+  <si>
+    <t>CMYK P 142-14 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 5545 CP</t>
+  </si>
+  <si>
+    <t>Color Bridge 3255 CP</t>
+  </si>
+  <si>
+    <t>Extended Gamut 318 XGC</t>
+  </si>
+  <si>
+    <t>Formular Guide 7456 C</t>
+  </si>
+  <si>
+    <t>CMYK P 126-5 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 339 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 2410 CP</t>
+  </si>
+  <si>
+    <t>Formular Guide 2360 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 645 C</t>
+  </si>
+  <si>
+    <t>CMYK P 179-1 C</t>
+  </si>
+  <si>
+    <t>Formular Guide Black 6 C</t>
+  </si>
+  <si>
+    <t>Extended Gamut 7539 XGC</t>
+  </si>
+  <si>
+    <t>Formular Guide Cool Gray
+6 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4292 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 8462 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7541 C</t>
+  </si>
+  <si>
+    <t>Pastels &amp; Neons 9142 C</t>
+  </si>
+  <si>
+    <t>CMYK P 3-1 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 468 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 683 C</t>
+  </si>
+  <si>
+    <t>CMYK P 81-15 C</t>
+  </si>
+  <si>
+    <t>Color Bridge Purple CP</t>
+  </si>
+  <si>
+    <t>Formular Guide 2082 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 5125 C</t>
+  </si>
+  <si>
+    <t>Extended Gamut 2090 XGC</t>
+  </si>
+  <si>
+    <t>Formular Guide 2114 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4121 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 666 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7617 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 695 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 7626 CP</t>
+  </si>
+  <si>
+    <t>Extended Gamut 198 XGC</t>
+  </si>
+  <si>
+    <t>Formular Guide 7608 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 499 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4715 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7515 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7618 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7416 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 1777 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7410 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 4095 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 3527 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7423 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 2045 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 218 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 508 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 509 C</t>
+  </si>
+  <si>
+    <t>Color Bridge 2033 CP</t>
+  </si>
+  <si>
+    <t>Formular Guide 2469 C</t>
+  </si>
+  <si>
+    <t>Formular Guide 7646 C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2024,6 +2289,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2033,12 +2305,42 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2047,9 +2349,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2365,18 +2673,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D027F-EF52-4720-8987-66F19777A7B6}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F1" sqref="F1:F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="7" width="14.25" customWidth="1"/>
+    <col min="1" max="5" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="17.5" thickBot="1">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -2392,14 +2702,17 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="17.5" thickBot="1">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -2415,14 +2728,17 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="17.5" thickBot="1">
       <c r="A3" t="s">
         <v>208</v>
       </c>
@@ -2438,14 +2754,17 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="17.5" thickBot="1">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -2461,11 +2780,14 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="17.5" thickBot="1">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -2481,11 +2803,14 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="17.5" thickBot="1">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -2501,11 +2826,14 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="17.5" thickBot="1">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -2521,11 +2849,14 @@
       <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="17.5" thickBot="1">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -2541,11 +2872,14 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="17.5" thickBot="1">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -2561,11 +2895,14 @@
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="17.5" thickBot="1">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -2581,11 +2918,14 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="17.5" thickBot="1">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -2601,11 +2941,14 @@
       <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="17.5" thickBot="1">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -2621,11 +2964,14 @@
       <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="17.5" thickBot="1">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -2641,11 +2987,14 @@
       <c r="E13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="17.5" thickBot="1">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -2661,11 +3010,14 @@
       <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="17.5" thickBot="1">
       <c r="A15" t="s">
         <v>292</v>
       </c>
@@ -2681,11 +3033,14 @@
       <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="H15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="17.5" thickBot="1">
       <c r="A16" t="s">
         <v>219</v>
       </c>
@@ -2701,11 +3056,14 @@
       <c r="E16" t="s">
         <v>53</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="17.5" thickBot="1">
       <c r="A17" t="s">
         <v>220</v>
       </c>
@@ -2721,11 +3079,14 @@
       <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="G17" t="s">
+      <c r="F17" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="17.5" thickBot="1">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -2741,11 +3102,14 @@
       <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F18" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="17.5" thickBot="1">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -2761,11 +3125,14 @@
       <c r="E19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" t="s">
+      <c r="F19" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="17.5" thickBot="1">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -2781,8 +3148,11 @@
       <c r="E20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F20" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17.5" thickBot="1">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -2798,8 +3168,11 @@
       <c r="E21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F21" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17.5" thickBot="1">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -2815,8 +3188,11 @@
       <c r="E22" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F22" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17.5" thickBot="1">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -2832,8 +3208,11 @@
       <c r="E23" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F23" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17.5" thickBot="1">
       <c r="A24" t="s">
         <v>227</v>
       </c>
@@ -2849,8 +3228,11 @@
       <c r="E24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F24" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17.5" thickBot="1">
       <c r="A25" t="s">
         <v>293</v>
       </c>
@@ -2866,8 +3248,11 @@
       <c r="E25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F25" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17.5" thickBot="1">
       <c r="A26" t="s">
         <v>228</v>
       </c>
@@ -2883,8 +3268,11 @@
       <c r="E26" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F26" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17.5" thickBot="1">
       <c r="A27" t="s">
         <v>229</v>
       </c>
@@ -2900,8 +3288,11 @@
       <c r="E27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F27" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17.5" thickBot="1">
       <c r="A28" t="s">
         <v>230</v>
       </c>
@@ -2917,8 +3308,11 @@
       <c r="E28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F28" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.5" thickBot="1">
       <c r="A29" t="s">
         <v>231</v>
       </c>
@@ -2934,8 +3328,11 @@
       <c r="E29" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F29" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17.5" thickBot="1">
       <c r="A30" t="s">
         <v>232</v>
       </c>
@@ -2951,8 +3348,11 @@
       <c r="E30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F30" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17.5" thickBot="1">
       <c r="A31" t="s">
         <v>233</v>
       </c>
@@ -2968,8 +3368,11 @@
       <c r="E31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F31" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17.5" thickBot="1">
       <c r="A32" t="s">
         <v>234</v>
       </c>
@@ -2985,8 +3388,11 @@
       <c r="E32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F32" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17.5" thickBot="1">
       <c r="A33" t="s">
         <v>235</v>
       </c>
@@ -3002,8 +3408,11 @@
       <c r="E33" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F33" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17.5" thickBot="1">
       <c r="A34" t="s">
         <v>236</v>
       </c>
@@ -3019,8 +3428,11 @@
       <c r="E34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F34" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17.5" thickBot="1">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -3036,8 +3448,11 @@
       <c r="E35" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17.5" thickBot="1">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -3053,8 +3468,11 @@
       <c r="E36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F36" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17.5" thickBot="1">
       <c r="A37" t="s">
         <v>239</v>
       </c>
@@ -3070,8 +3488,11 @@
       <c r="E37" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17.5" thickBot="1">
       <c r="A38" t="s">
         <v>240</v>
       </c>
@@ -3087,8 +3508,11 @@
       <c r="E38" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F38" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17.5" thickBot="1">
       <c r="A39" t="s">
         <v>241</v>
       </c>
@@ -3104,8 +3528,11 @@
       <c r="E39" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F39" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17.5" thickBot="1">
       <c r="A40" t="s">
         <v>242</v>
       </c>
@@ -3121,8 +3548,11 @@
       <c r="E40" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F40" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17.5" thickBot="1">
       <c r="A41" t="s">
         <v>243</v>
       </c>
@@ -3138,8 +3568,11 @@
       <c r="E41" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F41" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17.5" thickBot="1">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -3155,8 +3588,11 @@
       <c r="E42" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17.5" thickBot="1">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -3172,8 +3608,11 @@
       <c r="E43" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F43" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17.5" thickBot="1">
       <c r="A44" t="s">
         <v>246</v>
       </c>
@@ -3189,8 +3628,11 @@
       <c r="E44" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F44" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17.5" thickBot="1">
       <c r="A45" t="s">
         <v>247</v>
       </c>
@@ -3206,8 +3648,11 @@
       <c r="E45" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F45" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17.5" thickBot="1">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -3223,8 +3668,11 @@
       <c r="E46" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F46" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17.5" thickBot="1">
       <c r="A47" t="s">
         <v>249</v>
       </c>
@@ -3240,8 +3688,11 @@
       <c r="E47" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F47" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17.5" thickBot="1">
       <c r="A48" t="s">
         <v>250</v>
       </c>
@@ -3257,8 +3708,11 @@
       <c r="E48" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F48" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17.5" thickBot="1">
       <c r="A49" t="s">
         <v>251</v>
       </c>
@@ -3274,8 +3728,11 @@
       <c r="E49" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F49" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17.5" thickBot="1">
       <c r="A50" t="s">
         <v>252</v>
       </c>
@@ -3291,8 +3748,11 @@
       <c r="E50" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F50" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17.5" thickBot="1">
       <c r="A51" t="s">
         <v>253</v>
       </c>
@@ -3308,8 +3768,11 @@
       <c r="E51" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="34.5" thickBot="1">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -3325,8 +3788,11 @@
       <c r="E52" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17.5" thickBot="1">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -3342,8 +3808,11 @@
       <c r="E53" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17.5" thickBot="1">
       <c r="A54" t="s">
         <v>256</v>
       </c>
@@ -3359,8 +3828,11 @@
       <c r="E54" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="17.5" thickBot="1">
       <c r="A55" t="s">
         <v>257</v>
       </c>
@@ -3376,8 +3848,11 @@
       <c r="E55" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17.5" thickBot="1">
       <c r="A56" t="s">
         <v>258</v>
       </c>
@@ -3393,8 +3868,11 @@
       <c r="E56" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17.5" thickBot="1">
       <c r="A57" t="s">
         <v>259</v>
       </c>
@@ -3410,8 +3888,11 @@
       <c r="E57" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17.5" thickBot="1">
       <c r="A58" t="s">
         <v>260</v>
       </c>
@@ -3427,8 +3908,11 @@
       <c r="E58" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="17.5" thickBot="1">
       <c r="A59" t="s">
         <v>261</v>
       </c>
@@ -3444,8 +3928,11 @@
       <c r="E59" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="17.5" thickBot="1">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -3461,8 +3948,11 @@
       <c r="E60" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17.5" thickBot="1">
       <c r="A61" t="s">
         <v>263</v>
       </c>
@@ -3478,8 +3968,11 @@
       <c r="E61" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="17.5" thickBot="1">
       <c r="A62" t="s">
         <v>264</v>
       </c>
@@ -3495,8 +3988,11 @@
       <c r="E62" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F62" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17.5" thickBot="1">
       <c r="A63" t="s">
         <v>265</v>
       </c>
@@ -3512,8 +4008,11 @@
       <c r="E63" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F63" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17.5" thickBot="1">
       <c r="A64" t="s">
         <v>294</v>
       </c>
@@ -3529,8 +4028,11 @@
       <c r="E64" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F64" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17.5" thickBot="1">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -3546,8 +4048,11 @@
       <c r="E65" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F65" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17.5" thickBot="1">
       <c r="A66" t="s">
         <v>267</v>
       </c>
@@ -3563,8 +4068,11 @@
       <c r="E66" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17.5" thickBot="1">
       <c r="A67" t="s">
         <v>268</v>
       </c>
@@ -3580,8 +4088,11 @@
       <c r="E67" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F67" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17.5" thickBot="1">
       <c r="A68" t="s">
         <v>269</v>
       </c>
@@ -3597,8 +4108,11 @@
       <c r="E68" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F68" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17.5" thickBot="1">
       <c r="A69" t="s">
         <v>270</v>
       </c>
@@ -3614,8 +4128,11 @@
       <c r="E69" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F69" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="17.5" thickBot="1">
       <c r="A70" t="s">
         <v>271</v>
       </c>
@@ -3631,8 +4148,11 @@
       <c r="E70" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F70" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="17.5" thickBot="1">
       <c r="A71" t="s">
         <v>272</v>
       </c>
@@ -3648,8 +4168,11 @@
       <c r="E71" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="17.5" thickBot="1">
       <c r="A72" t="s">
         <v>273</v>
       </c>
@@ -3665,8 +4188,11 @@
       <c r="E72" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F72" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="17.5" thickBot="1">
       <c r="A73" t="s">
         <v>274</v>
       </c>
@@ -3682,8 +4208,11 @@
       <c r="E73" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F73" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="17.5" thickBot="1">
       <c r="A74" t="s">
         <v>275</v>
       </c>
@@ -3699,8 +4228,11 @@
       <c r="E74" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F74" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="17.5" thickBot="1">
       <c r="A75" t="s">
         <v>295</v>
       </c>
@@ -3716,8 +4248,11 @@
       <c r="E75" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F75" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="17.5" thickBot="1">
       <c r="A76" t="s">
         <v>276</v>
       </c>
@@ -3733,8 +4268,11 @@
       <c r="E76" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F76" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="17.5" thickBot="1">
       <c r="A77" t="s">
         <v>277</v>
       </c>
@@ -3750,8 +4288,11 @@
       <c r="E77" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F77" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17.5" thickBot="1">
       <c r="A78" t="s">
         <v>278</v>
       </c>
@@ -3767,8 +4308,11 @@
       <c r="E78" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F78" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17.5" thickBot="1">
       <c r="A79" t="s">
         <v>279</v>
       </c>
@@ -3784,8 +4328,11 @@
       <c r="E79" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F79" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="17.5" thickBot="1">
       <c r="A80" t="s">
         <v>280</v>
       </c>
@@ -3801,8 +4348,11 @@
       <c r="E80" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F80" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="17.5" thickBot="1">
       <c r="A81" t="s">
         <v>281</v>
       </c>
@@ -3818,8 +4368,11 @@
       <c r="E81" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F81" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="17.5" thickBot="1">
       <c r="A82" t="s">
         <v>282</v>
       </c>
@@ -3835,8 +4388,11 @@
       <c r="E82" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F82" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="17.5" thickBot="1">
       <c r="A83" t="s">
         <v>283</v>
       </c>
@@ -3852,8 +4408,11 @@
       <c r="E83" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F83" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="17.5" thickBot="1">
       <c r="A84" t="s">
         <v>284</v>
       </c>
@@ -3869,8 +4428,11 @@
       <c r="E84" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F84" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="17.5" thickBot="1">
       <c r="A85" t="s">
         <v>285</v>
       </c>
@@ -3886,8 +4448,11 @@
       <c r="E85" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F85" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="17.5" thickBot="1">
       <c r="A86" t="s">
         <v>286</v>
       </c>
@@ -3903,8 +4468,11 @@
       <c r="E86" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F86" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="17.5" thickBot="1">
       <c r="A87" t="s">
         <v>287</v>
       </c>
@@ -3920,8 +4488,11 @@
       <c r="E87" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F87" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="17.5" thickBot="1">
       <c r="A88" t="s">
         <v>288</v>
       </c>
@@ -3937,8 +4508,11 @@
       <c r="E88" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F88" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="17.5" thickBot="1">
       <c r="A89" t="s">
         <v>289</v>
       </c>
@@ -3954,8 +4528,11 @@
       <c r="E89" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F89" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="17.5" thickBot="1">
       <c r="A90" t="s">
         <v>290</v>
       </c>
@@ -3970,10 +4547,14 @@
       </c>
       <c r="E90" t="s">
         <v>205</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data add color xlsx
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagja\Desktop\DHS207_Introduction to Digital History\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6173F7A-19C7-4B4E-B1E6-BCB987C8B962}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4490E5F-BC18-412A-90D6-6FAA0A85DAC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9225" xr2:uid="{91E5F28C-6291-45D4-8C0D-F3DDD27ECA86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="606">
   <si>
     <t>#ecd437</t>
   </si>
@@ -2755,6 +2755,102 @@
   </si>
   <si>
     <t>백색;연람색;담자색;자색;회보라색;포도색;구색;다자색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;감색;청색;행황색;적색;두록색;흑청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구색;담자색;설백색;치색;자황색;백색;청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구색;담자색;백색;흑색;천청색;치색;회보라색;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;초록색;구색;흑색;담황색;옥색;천청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황색;홍황색;담황색;연두색;자황색;백색;뇌록색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담황색;연분홍색;백색;청벽색;회보라색;회색;비색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;적색;청색;유황색;보라색;연두색;뇌록색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황색;연두색;담황색;청색;백색;천청색;구색;흑록색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담황색;옥색;진분홍색;청색;분홍색;적색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥색;비색;진초록색;연두색;흑록색;백색;청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담황색;자색;백색;흑색;분홍색;자황색;보라색;청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;적황색;소색;자황색;벽자색;청록색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설백색;적색;백색;초록색;벽자색;소색;청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적색;청색;소색;구색;지황색;자색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황색;적색;자주색;청색;춘유록색;연두색;담황색;보라색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;자색;벽자색;흑색;회색;청색;적색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적색;청색;적황색;담황색;자황색;황색;진분홍색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;천청색;비색;흑색;구색;청색;연두색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;흑색;자황색;양록색;적색;회보라색;벽청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구색;흑색;분홍색;청색;백색;자황색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;흑색;토황색;석간주색;회색;홍람색;구색;청색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담황색;연두색;분홍색;진분홍색;지황색;흑색;구색;청자색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회보라색;남색;두록색;흑색;지황색;다자색;홍황색;양람색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황색;벽청색</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3139,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D027F-EF52-4720-8987-66F19777A7B6}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3670,6 +3766,9 @@
       <c r="G20" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="H20" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -3693,6 +3792,9 @@
       <c r="G21" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="H21" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -3716,6 +3818,9 @@
       <c r="G22" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="H22" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -3947,6 +4052,9 @@
       <c r="G31" s="1" t="s">
         <v>439</v>
       </c>
+      <c r="H31" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -3970,8 +4078,11 @@
       <c r="G32" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -3993,8 +4104,11 @@
       <c r="G33" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>209</v>
       </c>
@@ -4016,8 +4130,11 @@
       <c r="G34" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>210</v>
       </c>
@@ -4039,8 +4156,11 @@
       <c r="G35" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>211</v>
       </c>
@@ -4062,8 +4182,11 @@
       <c r="G36" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>212</v>
       </c>
@@ -4085,8 +4208,11 @@
       <c r="G37" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>213</v>
       </c>
@@ -4108,8 +4234,11 @@
       <c r="G38" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>214</v>
       </c>
@@ -4131,8 +4260,11 @@
       <c r="G39" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>215</v>
       </c>
@@ -4154,8 +4286,11 @@
       <c r="G40" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>216</v>
       </c>
@@ -4177,8 +4312,11 @@
       <c r="G41" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>217</v>
       </c>
@@ -4200,8 +4338,11 @@
       <c r="G42" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>218</v>
       </c>
@@ -4223,8 +4364,11 @@
       <c r="G43" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>219</v>
       </c>
@@ -4246,8 +4390,11 @@
       <c r="G44" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>220</v>
       </c>
@@ -4269,8 +4416,11 @@
       <c r="G45" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>221</v>
       </c>
@@ -4292,8 +4442,11 @@
       <c r="G46" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>222</v>
       </c>
@@ -4315,8 +4468,11 @@
       <c r="G47" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>223</v>
       </c>
@@ -4338,8 +4494,11 @@
       <c r="G48" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>224</v>
       </c>
@@ -4362,7 +4521,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -4385,7 +4544,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>226</v>
       </c>
@@ -4408,7 +4567,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>227</v>
       </c>
@@ -4431,7 +4590,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -4454,7 +4613,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>229</v>
       </c>
@@ -4477,7 +4636,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>230</v>
       </c>
@@ -4500,7 +4659,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -4523,7 +4682,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>232</v>
       </c>
@@ -4546,7 +4705,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>233</v>
       </c>
@@ -4569,7 +4728,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>234</v>
       </c>
@@ -4591,8 +4750,11 @@
       <c r="G59" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>235</v>
       </c>
@@ -4614,8 +4776,11 @@
       <c r="G60" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>236</v>
       </c>
@@ -4637,8 +4802,11 @@
       <c r="G61" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>237</v>
       </c>
@@ -4661,7 +4829,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>238</v>
       </c>
@@ -4684,7 +4852,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>435</v>
       </c>

</xml_diff>

<commit_message>
used with -finishted color.xlsx
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagja\Desktop\DHS207_Introduction to Digital History\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11647908-ED9B-4506-8A18-D4359CE08326}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102919FF-5AC1-4471-9054-814E5C742BE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9225" xr2:uid="{91E5F28C-6291-45D4-8C0D-F3DDD27ECA86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="625">
   <si>
     <t>#ecd437</t>
   </si>
@@ -2847,10 +2847,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>황색;벽청색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>黃色 천하를 통치하는 황제, 오행 중 토행이고 비옥하다. &lt;세종실록&gt; "임금이 영을 내려 황색에 가까운 복색과 서민의 단령의를 금하였다"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2903,7 +2899,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>백색;</t>
+    <t>백색;자황색;소색;홍황색;구색;연지회색;자황색;연두색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지백색;자황색;갈색;백색;연지회색;유황색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황색;벽청색;비색;청색;유록색;청자색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소색;치색;백색;청벽색;벽청색;흑색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백색;치색;벽자색;청색;군청색;명황색;적색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소색;다자색;회색;담자색;적색;구색;흑색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구색;흑색;백색;연지회색;청색;소색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두록색;회색;백색;자황색;적색;청색;흑청색</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3288,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D027F-EF52-4720-8987-66F19777A7B6}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3311,7 +3335,7 @@
         <v>372</v>
       </c>
       <c r="C1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -3337,7 +3361,7 @@
         <v>373</v>
       </c>
       <c r="C2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -4574,7 +4598,7 @@
         <v>440</v>
       </c>
       <c r="H49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -4599,6 +4623,9 @@
       <c r="G50" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H50" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -4622,6 +4649,9 @@
       <c r="G51" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H51" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -4645,6 +4675,9 @@
       <c r="G52" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H52" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -4668,6 +4701,9 @@
       <c r="G53" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H53" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -4691,6 +4727,9 @@
       <c r="G54" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H54" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -4715,7 +4754,7 @@
         <v>440</v>
       </c>
       <c r="H55" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -4741,7 +4780,7 @@
         <v>440</v>
       </c>
       <c r="H56" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -4767,7 +4806,7 @@
         <v>440</v>
       </c>
       <c r="H57" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -4792,6 +4831,9 @@
       <c r="G58" s="1" t="s">
         <v>440</v>
       </c>
+      <c r="H58" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -4868,7 +4910,7 @@
         <v>441</v>
       </c>
       <c r="H61" t="s">
-        <v>604</v>
+        <v>619</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -4894,7 +4936,7 @@
         <v>441</v>
       </c>
       <c r="H62" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -4920,7 +4962,7 @@
         <v>441</v>
       </c>
       <c r="H63" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -4946,7 +4988,7 @@
         <v>441</v>
       </c>
       <c r="H64" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -4972,7 +5014,7 @@
         <v>441</v>
       </c>
       <c r="H65" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -4998,7 +5040,7 @@
         <v>441</v>
       </c>
       <c r="H66" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -5024,7 +5066,7 @@
         <v>441</v>
       </c>
       <c r="H67" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -5050,7 +5092,7 @@
         <v>441</v>
       </c>
       <c r="H68" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -5076,7 +5118,7 @@
         <v>441</v>
       </c>
       <c r="H69" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="33" x14ac:dyDescent="0.3">

</xml_diff>